<commit_message>
Update to shipping fuel consumption
</commit_message>
<xml_diff>
--- a/input/energy/Shipping_Fuel_Consumption.xlsx
+++ b/input/energy/Shipping_Fuel_Consumption.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="18300" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="22620" windowHeight="18960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="References" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,8 +19,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Steve Smith</author>
+  </authors>
+  <commentList>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Times"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Times"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+"Bottom up" EstimatesThird IMO GHG Study 2014 (MEPC-67-6-INF3-2014).pdf</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E162" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Times"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Times"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Phase in small difference between estimates</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="34">
   <si>
     <t>Year</t>
   </si>
@@ -60,9 +119,6 @@
     <t>IMO 3d GHG Report</t>
   </si>
   <si>
-    <t>IMO Est Fuel Cons</t>
-  </si>
-  <si>
     <t>IMO "Bottom up"</t>
   </si>
   <si>
@@ -70,9 +126,6 @@
   </si>
   <si>
     <t>Source</t>
-  </si>
-  <si>
-    <t>Extrapoltion</t>
   </si>
   <si>
     <t>Smith et al. (2011)</t>
@@ -98,12 +151,42 @@
   <si>
     <t>Smith et al. ACP 11, 1101–1116 (2011) and adl sources as noted below</t>
   </si>
+  <si>
+    <t>Extrapolation</t>
+  </si>
+  <si>
+    <t>Smith et al. (2011) methodology</t>
+  </si>
+  <si>
+    <t>Fuel Estimates</t>
+  </si>
+  <si>
+    <t>IMO</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Endresen, Ø., Sørgard, E., Behrens, H.L., Brett, P.O., and Isak- sen, I.S.A.: A historical reconstruction of ships’ fuel con- sumption and emissions, J. Geophys. Res., 112, D12301, doi:10.1029/2006JD007630, 2007.</t>
+  </si>
+  <si>
+    <t>Eyring, V., Isaksen, I. S. A., Berntsen, T., Collins, W. J., Corbett, J. J., Endresen, O., Grainger, R. G., Moldanova, J., Schlager, H., and Stevenson, D. S.: Transport impacts on atmosphere and climate: Shipping, Atmos. Environ., 44, 4735–4771, 2010.</t>
+  </si>
+  <si>
+    <t>Fletcher, M. E.: “From coal to oil in British shipping” in: Williams, David, M., The World of Shipping, by Aldershot, Hants, Eng- land, Ashgate, Brookfield VT, 1997.</t>
+  </si>
+  <si>
+    <t>IMO (2014) Reduction of GHG Emissions From Ships: Third IMO GHG Study 2014 (MEPC-67-6-INF3-2014)</t>
+  </si>
+  <si>
+    <t>Smith, SJ, J van Aardenne, Z Klimont, R Andres, AC Volke, and S Delgado Arias (2011) Anthropogenic Sulfur Dioxide Emissions: 1850-2005 Atmos. Chem. Phys., 11, 1101–1116.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,6 +212,19 @@
       <name val="Times"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Times"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Times"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,14 +243,62 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -165,12 +309,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,42 +692,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FH16388"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G159" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:B3"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="164" width="9.33203125" customWidth="1"/>
+    <col min="2" max="11" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="164" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:164">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:164">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:164">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:164">
+      <c r="I4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:164">
@@ -560,19 +760,22 @@
         <v>7</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" t="s">
-        <v>16</v>
-      </c>
       <c r="O5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:164">
@@ -583,9 +786,11 @@
         <v>3257.7644104169722</v>
       </c>
       <c r="C6" s="1">
+        <f t="shared" ref="C6:C69" si="0">$E6*($L6)</f>
         <v>0</v>
       </c>
       <c r="D6" s="1">
+        <f t="shared" ref="D6:D69" si="1">$E6*(1-$L6)</f>
         <v>0</v>
       </c>
       <c r="E6" s="1">
@@ -601,7 +806,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -742,9 +947,11 @@
         <v>3572.5719507243793</v>
       </c>
       <c r="C7" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D7" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E7" s="1">
@@ -758,7 +965,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -917,9 +1124,11 @@
         <v>3887.3794910317861</v>
       </c>
       <c r="C8" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D8" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E8" s="1">
@@ -933,7 +1142,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1092,9 +1301,11 @@
         <v>4202.1870313391937</v>
       </c>
       <c r="C9" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D9" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E9" s="1">
@@ -1108,7 +1319,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1267,9 +1478,11 @@
         <v>4516.9945716466</v>
       </c>
       <c r="C10" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D10" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E10" s="1">
@@ -1283,7 +1496,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M10" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1442,9 +1655,11 @@
         <v>4831.8021119540072</v>
       </c>
       <c r="C11" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D11" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E11" s="1">
@@ -1461,7 +1676,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N11"/>
       <c r="O11"/>
@@ -1475,9 +1690,11 @@
         <v>5146.6096522614143</v>
       </c>
       <c r="C12" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D12" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E12" s="1">
@@ -1491,7 +1708,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:164">
@@ -1502,9 +1719,11 @@
         <v>5461.4171925688206</v>
       </c>
       <c r="C13" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D13" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -1518,7 +1737,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="FC13" s="1"/>
       <c r="FD13" s="1"/>
@@ -1535,9 +1754,11 @@
         <v>5776.2247328762278</v>
       </c>
       <c r="C14" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D14" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E14" s="1">
@@ -1551,7 +1772,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:164">
@@ -1562,9 +1783,11 @@
         <v>6091.032273183635</v>
       </c>
       <c r="C15" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D15" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E15" s="1">
@@ -1578,7 +1801,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M15" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:164">
@@ -1589,9 +1812,11 @@
         <v>6405.8398134910422</v>
       </c>
       <c r="C16" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D16" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E16" s="1">
@@ -1607,7 +1832,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1766,9 +1991,11 @@
         <v>6877.1157200783537</v>
       </c>
       <c r="C17" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D17" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E17" s="1">
@@ -1782,7 +2009,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:164">
@@ -1793,9 +2020,11 @@
         <v>7348.3916266656652</v>
       </c>
       <c r="C18" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D18" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E18" s="1">
@@ -1809,7 +2038,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:164">
@@ -1820,9 +2049,11 @@
         <v>7819.6675332529767</v>
       </c>
       <c r="C19" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D19" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E19" s="1">
@@ -1836,7 +2067,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M19" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="DR19" s="1"/>
       <c r="DS19" s="1"/>
@@ -1890,9 +2121,11 @@
         <v>8290.9434398402882</v>
       </c>
       <c r="C20" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D20" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E20" s="1">
@@ -1906,7 +2139,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M20" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:164">
@@ -1917,9 +2150,11 @@
         <v>8762.2193464275988</v>
       </c>
       <c r="C21" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D21" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E21" s="1">
@@ -1933,7 +2168,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M21" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:164">
@@ -1944,9 +2179,11 @@
         <v>9233.4952530149112</v>
       </c>
       <c r="C22" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D22" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E22" s="1">
@@ -1960,7 +2197,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M22" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:164">
@@ -1971,9 +2208,11 @@
         <v>9704.7711596022236</v>
       </c>
       <c r="C23" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D23" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E23" s="1">
@@ -1987,7 +2226,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M23" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:164">
@@ -1998,9 +2237,11 @@
         <v>10176.047066189534</v>
       </c>
       <c r="C24" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D24" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E24" s="1">
@@ -2014,7 +2255,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M24" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:164">
@@ -2025,9 +2266,11 @@
         <v>10647.322972776845</v>
       </c>
       <c r="C25" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D25" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E25" s="1">
@@ -2041,7 +2284,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:164">
@@ -2052,9 +2295,11 @@
         <v>11118.598879364157</v>
       </c>
       <c r="C26" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D26" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E26" s="1">
@@ -2070,7 +2315,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:164">
@@ -2081,9 +2326,11 @@
         <v>11956.738991427741</v>
       </c>
       <c r="C27" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D27" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E27" s="1">
@@ -2097,7 +2344,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M27" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:164">
@@ -2108,9 +2355,11 @@
         <v>12794.879103491327</v>
       </c>
       <c r="C28" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D28" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E28" s="1">
@@ -2124,7 +2373,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M28" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:164">
@@ -2135,9 +2384,11 @@
         <v>13633.01921555491</v>
       </c>
       <c r="C29" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D29" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E29" s="1">
@@ -2151,7 +2402,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M29" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:164">
@@ -2162,9 +2413,11 @@
         <v>14471.159327618494</v>
       </c>
       <c r="C30" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D30" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E30" s="1">
@@ -2178,7 +2431,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M30" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:164">
@@ -2189,9 +2442,11 @@
         <v>15309.29943968208</v>
       </c>
       <c r="C31" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D31" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E31" s="1">
@@ -2205,7 +2460,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M31" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:164">
@@ -2216,9 +2471,11 @@
         <v>16147.439551745663</v>
       </c>
       <c r="C32" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D32" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E32" s="1">
@@ -2232,7 +2489,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M32" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2243,9 +2500,11 @@
         <v>16985.579663809247</v>
       </c>
       <c r="C33" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D33" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E33" s="1">
@@ -2259,7 +2518,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M33" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -2270,9 +2529,11 @@
         <v>17823.719775872833</v>
       </c>
       <c r="C34" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D34" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E34" s="1">
@@ -2286,7 +2547,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M34" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2297,9 +2558,11 @@
         <v>18661.859887936414</v>
       </c>
       <c r="C35" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D35" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E35" s="1">
@@ -2313,7 +2576,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M35" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2324,9 +2587,11 @@
         <v>19500</v>
       </c>
       <c r="C36" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D36" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E36" s="1">
@@ -2342,7 +2607,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M36" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2353,9 +2618,11 @@
         <v>20690</v>
       </c>
       <c r="C37" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D37" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E37" s="1">
@@ -2369,7 +2636,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M37" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2380,9 +2647,11 @@
         <v>21880</v>
       </c>
       <c r="C38" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D38" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E38" s="1">
@@ -2396,7 +2665,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M38" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2407,9 +2676,11 @@
         <v>23070</v>
       </c>
       <c r="C39" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D39" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E39" s="1">
@@ -2423,7 +2694,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M39" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2434,9 +2705,11 @@
         <v>24260</v>
       </c>
       <c r="C40" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D40" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E40" s="1">
@@ -2450,7 +2723,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M40" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2461,9 +2734,11 @@
         <v>25450</v>
       </c>
       <c r="C41" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D41" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E41" s="1">
@@ -2477,7 +2752,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M41" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2488,9 +2763,11 @@
         <v>26640</v>
       </c>
       <c r="C42" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D42" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E42" s="1">
@@ -2504,7 +2781,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M42" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2515,9 +2792,11 @@
         <v>27830</v>
       </c>
       <c r="C43" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D43" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E43" s="1">
@@ -2531,7 +2810,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M43" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2542,9 +2821,11 @@
         <v>29020</v>
       </c>
       <c r="C44" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D44" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E44" s="1">
@@ -2558,7 +2839,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M44" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2569,9 +2850,11 @@
         <v>30210</v>
       </c>
       <c r="C45" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D45" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E45" s="1">
@@ -2585,7 +2868,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M45" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2596,9 +2879,11 @@
         <v>31400</v>
       </c>
       <c r="C46" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D46" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E46" s="1">
@@ -2614,7 +2899,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M46" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2625,9 +2910,11 @@
         <v>33030</v>
       </c>
       <c r="C47" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D47" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E47" s="1">
@@ -2641,7 +2928,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M47" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2652,9 +2939,11 @@
         <v>34660</v>
       </c>
       <c r="C48" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D48" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E48" s="1">
@@ -2668,7 +2957,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M48" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -2679,9 +2968,11 @@
         <v>36290</v>
       </c>
       <c r="C49" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D49" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E49" s="1">
@@ -2695,7 +2986,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M49" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -2706,9 +2997,11 @@
         <v>37920</v>
       </c>
       <c r="C50" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D50" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E50" s="1">
@@ -2722,7 +3015,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M50" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -2733,9 +3026,11 @@
         <v>39550</v>
       </c>
       <c r="C51" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D51" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E51" s="1">
@@ -2749,7 +3044,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M51" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -2760,9 +3055,11 @@
         <v>41180</v>
       </c>
       <c r="C52" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D52" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E52" s="1">
@@ -2776,7 +3073,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M52" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -2787,9 +3084,11 @@
         <v>42810</v>
       </c>
       <c r="C53" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D53" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E53" s="1">
@@ -2803,7 +3102,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M53" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -2814,9 +3113,11 @@
         <v>44440</v>
       </c>
       <c r="C54" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D54" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E54" s="1">
@@ -2830,7 +3131,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M54" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -2841,9 +3142,11 @@
         <v>46070</v>
       </c>
       <c r="C55" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D55" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E55" s="1">
@@ -2857,7 +3160,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M55" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -2868,9 +3171,11 @@
         <v>47700</v>
       </c>
       <c r="C56" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D56" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E56" s="1">
@@ -2886,7 +3191,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M56" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -2897,9 +3202,11 @@
         <v>50184.615384615383</v>
       </c>
       <c r="C57" s="1">
+        <f t="shared" si="0"/>
         <v>171.70693133152432</v>
       </c>
       <c r="D57" s="1">
+        <f t="shared" si="1"/>
         <v>44.888067872170545</v>
       </c>
       <c r="E57" s="1">
@@ -2913,7 +3220,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M57" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -2924,9 +3231,11 @@
         <v>52669.230769230766</v>
       </c>
       <c r="C58" s="1">
+        <f t="shared" si="0"/>
         <v>343.41386266304863</v>
       </c>
       <c r="D58" s="1">
+        <f t="shared" si="1"/>
         <v>89.77613574434109</v>
       </c>
       <c r="E58" s="1">
@@ -2940,7 +3249,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M58" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -2951,9 +3260,11 @@
         <v>55153.846153846156</v>
       </c>
       <c r="C59" s="1">
+        <f t="shared" si="0"/>
         <v>515.12079399457298</v>
       </c>
       <c r="D59" s="1">
+        <f t="shared" si="1"/>
         <v>134.66420361651163</v>
       </c>
       <c r="E59" s="1">
@@ -2967,7 +3278,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M59" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -2978,9 +3289,11 @@
         <v>57638.461538461539</v>
       </c>
       <c r="C60" s="1">
+        <f t="shared" si="0"/>
         <v>686.82772532609727</v>
       </c>
       <c r="D60" s="1">
+        <f t="shared" si="1"/>
         <v>179.55227148868218</v>
       </c>
       <c r="E60" s="1">
@@ -2994,7 +3307,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M60" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -3005,9 +3318,11 @@
         <v>60123.076923076922</v>
       </c>
       <c r="C61" s="1">
+        <f t="shared" si="0"/>
         <v>858.53465665762155</v>
       </c>
       <c r="D61" s="1">
+        <f t="shared" si="1"/>
         <v>224.4403393608527</v>
       </c>
       <c r="E61" s="1">
@@ -3021,7 +3336,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M61" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -3032,9 +3347,11 @@
         <v>62607.692307692312</v>
       </c>
       <c r="C62" s="1">
+        <f t="shared" si="0"/>
         <v>1030.241587989146</v>
       </c>
       <c r="D62" s="1">
+        <f t="shared" si="1"/>
         <v>269.32840723302326</v>
       </c>
       <c r="E62" s="1">
@@ -3048,7 +3365,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M62" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -3059,9 +3376,11 @@
         <v>65092.307692307695</v>
       </c>
       <c r="C63" s="1">
+        <f t="shared" si="0"/>
         <v>1201.9485193206704</v>
       </c>
       <c r="D63" s="1">
+        <f t="shared" si="1"/>
         <v>314.21647510519381</v>
       </c>
       <c r="E63" s="1">
@@ -3075,7 +3394,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M63" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -3086,9 +3405,11 @@
         <v>67576.923076923078</v>
       </c>
       <c r="C64" s="1">
+        <f t="shared" si="0"/>
         <v>1373.6554506521945</v>
       </c>
       <c r="D64" s="1">
+        <f t="shared" si="1"/>
         <v>359.10454297736436</v>
       </c>
       <c r="E64" s="1">
@@ -3102,7 +3423,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M64" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -3113,9 +3434,11 @@
         <v>70061.538461538468</v>
       </c>
       <c r="C65" s="1">
+        <f t="shared" si="0"/>
         <v>1545.3623819837189</v>
       </c>
       <c r="D65" s="1">
+        <f t="shared" si="1"/>
         <v>403.99261084953491</v>
       </c>
       <c r="E65" s="1">
@@ -3129,7 +3452,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M65" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -3140,9 +3463,11 @@
         <v>72546.153846153844</v>
       </c>
       <c r="C66" s="1">
+        <f t="shared" si="0"/>
         <v>1717.0693133152431</v>
       </c>
       <c r="D66" s="1">
+        <f t="shared" si="1"/>
         <v>448.88067872170541</v>
       </c>
       <c r="E66" s="1">
@@ -3156,7 +3481,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M66" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:13">
@@ -3167,9 +3492,11 @@
         <v>75030.769230769234</v>
       </c>
       <c r="C67" s="1">
+        <f t="shared" si="0"/>
         <v>1888.7762446467675</v>
       </c>
       <c r="D67" s="1">
+        <f t="shared" si="1"/>
         <v>493.76874659387596</v>
       </c>
       <c r="E67" s="1">
@@ -3183,7 +3510,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M67" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -3194,9 +3521,11 @@
         <v>77515.384615384624</v>
       </c>
       <c r="C68" s="1">
+        <f t="shared" si="0"/>
         <v>2060.4831759782919</v>
       </c>
       <c r="D68" s="1">
+        <f t="shared" si="1"/>
         <v>538.65681446604651</v>
       </c>
       <c r="E68" s="1">
@@ -3210,7 +3539,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M68" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -3221,9 +3550,11 @@
         <v>80000</v>
       </c>
       <c r="C69" s="1">
+        <f t="shared" si="0"/>
         <v>2232.1901073098161</v>
       </c>
       <c r="D69" s="1">
+        <f t="shared" si="1"/>
         <v>583.54488233821701</v>
       </c>
       <c r="E69" s="1">
@@ -3239,7 +3570,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M69" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -3250,9 +3581,11 @@
         <v>78225.185185185182</v>
       </c>
       <c r="C70" s="1">
+        <f t="shared" ref="C70:C133" si="2">$E70*($L70)</f>
         <v>3668.2406162604084</v>
       </c>
       <c r="D70" s="1">
+        <f t="shared" ref="D70:D133" si="3">$E70*(1-$L70)</f>
         <v>958.96090202806693</v>
       </c>
       <c r="E70" s="1">
@@ -3266,7 +3599,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M70" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -3277,9 +3610,11 @@
         <v>76450.370370370365</v>
       </c>
       <c r="C71" s="1">
+        <f t="shared" si="2"/>
         <v>5104.2911252109998</v>
       </c>
       <c r="D71" s="1">
+        <f t="shared" si="3"/>
         <v>1334.3769217179167</v>
       </c>
       <c r="E71" s="1">
@@ -3293,7 +3628,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M71" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:13">
@@ -3304,9 +3639,11 @@
         <v>74675.555555555562</v>
       </c>
       <c r="C72" s="1">
+        <f t="shared" si="2"/>
         <v>6540.3416341615921</v>
       </c>
       <c r="D72" s="1">
+        <f t="shared" si="3"/>
         <v>1709.7929414077664</v>
       </c>
       <c r="E72" s="1">
@@ -3320,7 +3657,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M72" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:13">
@@ -3331,9 +3668,11 @@
         <v>72900.740740740745</v>
       </c>
       <c r="C73" s="1">
+        <f t="shared" si="2"/>
         <v>7976.3921431121835</v>
       </c>
       <c r="D73" s="1">
+        <f t="shared" si="3"/>
         <v>2085.2089610976163</v>
       </c>
       <c r="E73" s="1">
@@ -3347,7 +3686,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M73" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:13">
@@ -3358,9 +3697,11 @@
         <v>71125.925925925927</v>
       </c>
       <c r="C74" s="1">
+        <f t="shared" si="2"/>
         <v>9412.4426520627749</v>
       </c>
       <c r="D74" s="1">
+        <f t="shared" si="3"/>
         <v>2460.624980787466</v>
       </c>
       <c r="E74" s="1">
@@ -3374,7 +3715,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M74" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:13">
@@ -3385,9 +3726,11 @@
         <v>69351.111111111109</v>
       </c>
       <c r="C75" s="1">
+        <f t="shared" si="2"/>
         <v>10848.493161013368</v>
       </c>
       <c r="D75" s="1">
+        <f t="shared" si="3"/>
         <v>2836.0410004773157</v>
       </c>
       <c r="E75" s="1">
@@ -3401,7 +3744,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M75" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -3412,9 +3755,11 @@
         <v>67576.296296296292</v>
       </c>
       <c r="C76" s="1">
+        <f t="shared" si="2"/>
         <v>12284.543669963959</v>
       </c>
       <c r="D76" s="1">
+        <f t="shared" si="3"/>
         <v>3211.4570201671654</v>
       </c>
       <c r="E76" s="1">
@@ -3428,7 +3773,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M76" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:13">
@@ -3439,9 +3784,11 @@
         <v>65801.481481481474</v>
       </c>
       <c r="C77" s="1">
+        <f t="shared" si="2"/>
         <v>13720.594178914551</v>
       </c>
       <c r="D77" s="1">
+        <f t="shared" si="3"/>
         <v>3586.8730398570151</v>
       </c>
       <c r="E77" s="1">
@@ -3455,7 +3802,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M77" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:13">
@@ -3466,9 +3813,11 @@
         <v>64026.666666666664</v>
       </c>
       <c r="C78" s="1">
+        <f t="shared" si="2"/>
         <v>15156.644687865142</v>
       </c>
       <c r="D78" s="1">
+        <f t="shared" si="3"/>
         <v>3962.2890595468648</v>
       </c>
       <c r="E78" s="1">
@@ -3482,7 +3831,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M78" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -3493,9 +3842,11 @@
         <v>62251.851851851854</v>
       </c>
       <c r="C79" s="1">
+        <f t="shared" si="2"/>
         <v>16592.695196815734</v>
       </c>
       <c r="D79" s="1">
+        <f t="shared" si="3"/>
         <v>4337.7050792367145</v>
       </c>
       <c r="E79" s="1">
@@ -3509,7 +3860,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M79" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -3520,9 +3871,11 @@
         <v>60477.037037037036</v>
       </c>
       <c r="C80" s="1">
+        <f t="shared" si="2"/>
         <v>18028.745705766327</v>
       </c>
       <c r="D80" s="1">
+        <f t="shared" si="3"/>
         <v>4713.1210989265646</v>
       </c>
       <c r="E80" s="1">
@@ -3536,7 +3889,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M80" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -3547,9 +3900,11 @@
         <v>58702.222222222219</v>
       </c>
       <c r="C81" s="1">
+        <f t="shared" si="2"/>
         <v>19464.796214716916</v>
       </c>
       <c r="D81" s="1">
+        <f t="shared" si="3"/>
         <v>5088.5371186164139</v>
       </c>
       <c r="E81" s="1">
@@ -3565,7 +3920,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M81" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -3576,9 +3931,11 @@
         <v>58490.555555555555</v>
       </c>
       <c r="C82" s="1">
+        <f t="shared" si="2"/>
         <v>20723.295969978786</v>
       </c>
       <c r="D82" s="1">
+        <f t="shared" si="3"/>
         <v>5417.5373633545441</v>
       </c>
       <c r="E82" s="1">
@@ -3592,7 +3949,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M82" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:13">
@@ -3603,9 +3960,11 @@
         <v>58278.888888888891</v>
       </c>
       <c r="C83" s="1">
+        <f t="shared" si="2"/>
         <v>21981.795725240656</v>
       </c>
       <c r="D83" s="1">
+        <f t="shared" si="3"/>
         <v>5746.5376080926744</v>
       </c>
       <c r="E83" s="1">
@@ -3619,7 +3978,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M83" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:13">
@@ -3630,9 +3989,11 @@
         <v>58067.222222222219</v>
       </c>
       <c r="C84" s="1">
+        <f t="shared" si="2"/>
         <v>23240.295480502526</v>
       </c>
       <c r="D84" s="1">
+        <f t="shared" si="3"/>
         <v>6075.5378528308047</v>
       </c>
       <c r="E84" s="1">
@@ -3646,7 +4007,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M84" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:13">
@@ -3657,9 +4018,11 @@
         <v>57855.555555555555</v>
       </c>
       <c r="C85" s="1">
+        <f t="shared" si="2"/>
         <v>24498.795235764395</v>
       </c>
       <c r="D85" s="1">
+        <f t="shared" si="3"/>
         <v>6404.538097568935</v>
       </c>
       <c r="E85" s="1">
@@ -3675,7 +4038,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M85" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -3686,9 +4049,11 @@
         <v>53198.888888888891</v>
       </c>
       <c r="C86" s="1">
+        <f t="shared" si="2"/>
         <v>23715.728721379233</v>
       </c>
       <c r="D86" s="1">
+        <f t="shared" si="3"/>
         <v>6199.8268341763205</v>
       </c>
       <c r="E86" s="1">
@@ -3702,7 +4067,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M86" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:13">
@@ -3713,9 +4078,11 @@
         <v>48542.222222222226</v>
       </c>
       <c r="C87" s="1">
+        <f t="shared" si="2"/>
         <v>22932.662206994071</v>
       </c>
       <c r="D87" s="1">
+        <f t="shared" si="3"/>
         <v>5995.115570783707</v>
       </c>
       <c r="E87" s="1">
@@ -3729,7 +4096,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M87" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:13">
@@ -3740,9 +4107,11 @@
         <v>43885.555555555562</v>
       </c>
       <c r="C88" s="1">
+        <f t="shared" si="2"/>
         <v>22149.595692608909</v>
       </c>
       <c r="D88" s="1">
+        <f t="shared" si="3"/>
         <v>5790.4043073910925</v>
       </c>
       <c r="E88" s="1">
@@ -3756,7 +4125,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M88" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:13">
@@ -3767,9 +4136,11 @@
         <v>39228.888888888898</v>
       </c>
       <c r="C89" s="1">
+        <f t="shared" si="2"/>
         <v>21366.529178223744</v>
       </c>
       <c r="D89" s="1">
+        <f t="shared" si="3"/>
         <v>5585.6930439984781</v>
       </c>
       <c r="E89" s="1">
@@ -3785,7 +4156,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M89" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -3796,9 +4167,11 @@
         <v>40251.944444444453</v>
       </c>
       <c r="C90" s="1">
+        <f t="shared" si="2"/>
         <v>22625.028933485613</v>
       </c>
       <c r="D90" s="1">
+        <f t="shared" si="3"/>
         <v>5914.6932887366083</v>
       </c>
       <c r="E90" s="1">
@@ -3812,7 +4185,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M90" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:13">
@@ -3823,9 +4196,11 @@
         <v>41275</v>
       </c>
       <c r="C91" s="1">
+        <f t="shared" si="2"/>
         <v>23883.528688747479</v>
       </c>
       <c r="D91" s="1">
+        <f t="shared" si="3"/>
         <v>6243.6935334747377</v>
       </c>
       <c r="E91" s="1">
@@ -3839,7 +4214,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M91" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:13">
@@ -3850,9 +4225,11 @@
         <v>42298.055555555555</v>
       </c>
       <c r="C92" s="1">
+        <f t="shared" si="2"/>
         <v>25142.028444009353</v>
       </c>
       <c r="D92" s="1">
+        <f t="shared" si="3"/>
         <v>6572.693778212868</v>
       </c>
       <c r="E92" s="1">
@@ -3866,7 +4243,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M92" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:13">
@@ -3877,9 +4254,11 @@
         <v>43321.111111111109</v>
       </c>
       <c r="C93" s="1">
+        <f t="shared" si="2"/>
         <v>26400.528199271223</v>
       </c>
       <c r="D93" s="1">
+        <f t="shared" si="3"/>
         <v>6901.6940229509983</v>
       </c>
       <c r="E93" s="1">
@@ -3895,7 +4274,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M93" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:13">
@@ -3906,9 +4285,11 @@
         <v>39511.111111111109</v>
       </c>
       <c r="C94" s="1">
+        <f t="shared" si="2"/>
         <v>23939.462011203563</v>
       </c>
       <c r="D94" s="1">
+        <f t="shared" si="3"/>
         <v>6258.3157665742101</v>
       </c>
       <c r="E94" s="1">
@@ -3924,7 +4305,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M94" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:13">
@@ -3935,9 +4316,11 @@
         <v>37653.148148148146</v>
       </c>
       <c r="C95" s="1">
+        <f t="shared" si="2"/>
         <v>26465.783742136646</v>
       </c>
       <c r="D95" s="1">
+        <f t="shared" si="3"/>
         <v>6918.7532949003817</v>
       </c>
       <c r="E95" s="1">
@@ -3951,7 +4334,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M95" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:13">
@@ -3962,9 +4345,11 @@
         <v>35795.185185185182</v>
       </c>
       <c r="C96" s="1">
+        <f t="shared" si="2"/>
         <v>28992.105473069736</v>
       </c>
       <c r="D96" s="1">
+        <f t="shared" si="3"/>
         <v>7579.190823226555</v>
       </c>
       <c r="E96" s="1">
@@ -3978,7 +4363,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M96" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:13">
@@ -3989,9 +4374,11 @@
         <v>33937.222222222219</v>
       </c>
       <c r="C97" s="1">
+        <f t="shared" si="2"/>
         <v>31518.427204002819</v>
       </c>
       <c r="D97" s="1">
+        <f t="shared" si="3"/>
         <v>8239.6283515527266</v>
       </c>
       <c r="E97" s="1">
@@ -4005,7 +4392,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M97" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:13">
@@ -4016,9 +4403,11 @@
         <v>32079.259259259259</v>
       </c>
       <c r="C98" s="1">
+        <f t="shared" si="2"/>
         <v>34044.748934935909</v>
       </c>
       <c r="D98" s="1">
+        <f t="shared" si="3"/>
         <v>8900.0658798789009</v>
       </c>
       <c r="E98" s="1">
@@ -4032,7 +4421,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M98" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:13">
@@ -4043,9 +4432,11 @@
         <v>30221.296296296296</v>
       </c>
       <c r="C99" s="1">
+        <f t="shared" si="2"/>
         <v>36571.070665868996</v>
       </c>
       <c r="D99" s="1">
+        <f t="shared" si="3"/>
         <v>9560.5034082050715</v>
       </c>
       <c r="E99" s="1">
@@ -4059,7 +4450,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M99" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:13">
@@ -4070,9 +4461,11 @@
         <v>28363.333333333332</v>
       </c>
       <c r="C100" s="1">
+        <f t="shared" si="2"/>
         <v>39097.392396802083</v>
       </c>
       <c r="D100" s="1">
+        <f t="shared" si="3"/>
         <v>10220.940936531246</v>
       </c>
       <c r="E100" s="1">
@@ -4086,7 +4479,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M100" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="101" spans="1:13">
@@ -4097,9 +4490,11 @@
         <v>26505.370370370372</v>
       </c>
       <c r="C101" s="1">
+        <f t="shared" si="2"/>
         <v>41623.714127735169</v>
       </c>
       <c r="D101" s="1">
+        <f t="shared" si="3"/>
         <v>10881.378464857416</v>
       </c>
       <c r="E101" s="1">
@@ -4113,7 +4508,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M101" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:13">
@@ -4124,9 +4519,11 @@
         <v>24647.407407407409</v>
       </c>
       <c r="C102" s="1">
+        <f t="shared" si="2"/>
         <v>44150.035858668249</v>
       </c>
       <c r="D102" s="1">
+        <f t="shared" si="3"/>
         <v>11541.815993183589</v>
       </c>
       <c r="E102" s="1">
@@ -4140,7 +4537,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M102" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:13">
@@ -4151,9 +4548,11 @@
         <v>22789.444444444445</v>
       </c>
       <c r="C103" s="1">
+        <f t="shared" si="2"/>
         <v>46676.357589601343</v>
       </c>
       <c r="D103" s="1">
+        <f t="shared" si="3"/>
         <v>12202.253521509761</v>
       </c>
       <c r="E103" s="1">
@@ -4167,7 +4566,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M103" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -4178,9 +4577,11 @@
         <v>20931.481481481482</v>
       </c>
       <c r="C104" s="1">
+        <f t="shared" si="2"/>
         <v>49202.679320534429</v>
       </c>
       <c r="D104" s="1">
+        <f t="shared" si="3"/>
         <v>12862.691049835936</v>
       </c>
       <c r="E104" s="1">
@@ -4194,7 +4595,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M104" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:13">
@@ -4205,9 +4606,11 @@
         <v>19073.518518518518</v>
       </c>
       <c r="C105" s="1">
+        <f t="shared" si="2"/>
         <v>51729.001051467516</v>
       </c>
       <c r="D105" s="1">
+        <f t="shared" si="3"/>
         <v>13523.128578162106</v>
       </c>
       <c r="E105" s="1">
@@ -4221,7 +4624,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M105" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -4232,9 +4635,11 @@
         <v>17215.555555555555</v>
       </c>
       <c r="C106" s="1">
+        <f t="shared" si="2"/>
         <v>54255.322782400595</v>
       </c>
       <c r="D106" s="1">
+        <f t="shared" si="3"/>
         <v>14183.566106488279</v>
       </c>
       <c r="E106" s="1">
@@ -4250,7 +4655,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M106" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -4261,9 +4666,11 @@
         <v>12925.777777777777</v>
       </c>
       <c r="C107" s="1">
+        <f t="shared" si="2"/>
         <v>53584.122912927611</v>
       </c>
       <c r="D107" s="1">
+        <f t="shared" si="3"/>
         <v>14008.099309294612</v>
       </c>
       <c r="E107" s="1">
@@ -4279,7 +4686,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M107" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:13">
@@ -4290,9 +4697,11 @@
         <v>10950.222222222221</v>
       </c>
       <c r="C108" s="1">
+        <f t="shared" si="2"/>
         <v>56716.388970468273</v>
       </c>
       <c r="D108" s="1">
+        <f t="shared" si="3"/>
         <v>14826.944362865072</v>
       </c>
       <c r="E108" s="1">
@@ -4308,7 +4717,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M108" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:13">
@@ -4319,9 +4728,11 @@
         <v>8692.4444444444434</v>
       </c>
       <c r="C109" s="1">
+        <f t="shared" si="2"/>
         <v>59177.455158535908</v>
       </c>
       <c r="D109" s="1">
+        <f t="shared" si="3"/>
         <v>15470.322619241855</v>
       </c>
       <c r="E109" s="1">
@@ -4337,7 +4748,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M109" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110" spans="1:13">
@@ -4348,9 +4759,11 @@
         <v>8043.3333333333348</v>
       </c>
       <c r="C110" s="1">
+        <f t="shared" si="2"/>
         <v>60296.12160765758</v>
       </c>
       <c r="D110" s="1">
+        <f t="shared" si="3"/>
         <v>15762.767281231307</v>
       </c>
       <c r="E110" s="1">
@@ -4366,7 +4779,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M110" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:13">
@@ -4377,9 +4790,11 @@
         <v>7549.4444444444434</v>
       </c>
       <c r="C111" s="1">
+        <f t="shared" si="2"/>
         <v>67455.586882036223</v>
       </c>
       <c r="D111" s="1">
+        <f t="shared" si="3"/>
         <v>17634.413117963781</v>
       </c>
       <c r="E111" s="1">
@@ -4395,7 +4810,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M111" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:13">
@@ -4406,9 +4821,11 @@
         <v>6307.6666666666661</v>
       </c>
       <c r="C112" s="1">
+        <f t="shared" si="2"/>
         <v>74615.052156414866</v>
       </c>
       <c r="D112" s="1">
+        <f t="shared" si="3"/>
         <v>19506.058954696258</v>
       </c>
       <c r="E112" s="1">
@@ -4424,7 +4841,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M112" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:16">
@@ -4435,9 +4852,11 @@
         <v>5362.2222222222217</v>
       </c>
       <c r="C113" s="1">
+        <f t="shared" si="2"/>
         <v>80543.984336759662</v>
       </c>
       <c r="D113" s="1">
+        <f t="shared" si="3"/>
         <v>21056.015663240334</v>
       </c>
       <c r="E113" s="1">
@@ -4453,7 +4872,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M113" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:16">
@@ -4464,9 +4883,11 @@
         <v>4035.7777777777778</v>
       </c>
       <c r="C114" s="1">
+        <f t="shared" si="2"/>
         <v>77076.118344482529</v>
       </c>
       <c r="D114" s="1">
+        <f t="shared" si="3"/>
         <v>20149.437211073047</v>
       </c>
       <c r="E114" s="1">
@@ -4482,7 +4903,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M114" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:16">
@@ -4493,9 +4914,11 @@
         <v>3132.666666666667</v>
       </c>
       <c r="C115" s="1">
+        <f t="shared" si="2"/>
         <v>77299.851634306833</v>
       </c>
       <c r="D115" s="1">
+        <f t="shared" si="3"/>
         <v>20207.92614347093</v>
       </c>
       <c r="E115" s="1">
@@ -4511,7 +4934,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M115" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:16">
@@ -4522,9 +4945,11 @@
         <v>2257.7777777777778</v>
       </c>
       <c r="C116" s="1">
+        <f t="shared" si="2"/>
         <v>86025.449937455822</v>
       </c>
       <c r="D116" s="1">
+        <f t="shared" si="3"/>
         <v>22488.994506988638</v>
       </c>
       <c r="E116" s="1">
@@ -4540,7 +4965,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M116" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:16">
@@ -4551,9 +4976,11 @@
         <v>1524</v>
       </c>
       <c r="C117" s="1">
+        <f t="shared" si="2"/>
         <v>94415.448305868282</v>
       </c>
       <c r="D117" s="1">
+        <f t="shared" si="3"/>
         <v>24682.329471909507</v>
       </c>
       <c r="E117" s="1">
@@ -4569,7 +4996,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M117" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:16">
@@ -4580,9 +5007,11 @@
         <v>1114.7777777777778</v>
       </c>
       <c r="C118" s="1">
+        <f t="shared" si="2"/>
         <v>95645.981399902099</v>
       </c>
       <c r="D118" s="1">
+        <f t="shared" si="3"/>
         <v>25004.018600097897</v>
       </c>
       <c r="E118" s="1">
@@ -4598,7 +5027,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M118" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:16">
@@ -4609,9 +5038,11 @@
         <v>987.7777777777776</v>
       </c>
       <c r="C119" s="1">
+        <f t="shared" si="2"/>
         <v>100232.5138413009</v>
       </c>
       <c r="D119" s="1">
+        <f t="shared" si="3"/>
         <v>26203.041714254636</v>
       </c>
       <c r="E119" s="1">
@@ -4627,7 +5058,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M119" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:16">
@@ -4638,9 +5069,11 @@
         <v>1114.7777777777778</v>
       </c>
       <c r="C120" s="1">
+        <f t="shared" si="2"/>
         <v>109069.97878936205</v>
       </c>
       <c r="D120" s="1">
+        <f t="shared" si="3"/>
         <v>28513.354543971291</v>
       </c>
       <c r="E120" s="1">
@@ -4656,7 +5089,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M120" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:16">
@@ -4667,9 +5100,11 @@
         <v>987.7777777777776</v>
       </c>
       <c r="C121" s="1">
+        <f t="shared" si="2"/>
         <v>113656.51123076085</v>
       </c>
       <c r="D121" s="1">
+        <f t="shared" si="3"/>
         <v>29712.377658128025</v>
       </c>
       <c r="E121" s="1">
@@ -4685,7 +5120,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M121" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:16">
@@ -4696,9 +5131,11 @@
         <v>1001.8888888888888</v>
       </c>
       <c r="C122" s="1">
+        <f t="shared" si="2"/>
         <v>108846.24549953772</v>
       </c>
       <c r="D122" s="1">
+        <f t="shared" si="3"/>
         <v>28454.865611573401</v>
       </c>
       <c r="E122" s="1">
@@ -4714,7 +5151,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M122" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" spans="1:16">
@@ -4725,9 +5162,11 @@
         <v>719.66666666666663</v>
       </c>
       <c r="C123" s="1">
+        <f t="shared" si="2"/>
         <v>117459.9771577745</v>
       </c>
       <c r="D123" s="1">
+        <f t="shared" si="3"/>
         <v>30706.689508892156</v>
       </c>
       <c r="E123" s="1">
@@ -4743,7 +5182,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M123" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:16">
@@ -4754,9 +5193,11 @@
         <v>437.4444444444444</v>
       </c>
       <c r="C124" s="1">
+        <f t="shared" si="2"/>
         <v>124843.17572197747</v>
       </c>
       <c r="D124" s="1">
+        <f t="shared" si="3"/>
         <v>32636.824278022519</v>
       </c>
       <c r="E124" s="1">
@@ -4772,7 +5213,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M124" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:16">
@@ -4783,9 +5224,11 @@
         <v>465.66666666666669</v>
       </c>
       <c r="C125" s="1">
+        <f t="shared" si="2"/>
         <v>114551.4443900582</v>
       </c>
       <c r="D125" s="1">
+        <f t="shared" si="3"/>
         <v>29946.333387719587</v>
       </c>
       <c r="E125" s="1">
@@ -4801,7 +5244,7 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M125" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:16">
@@ -4812,9 +5255,11 @@
         <v>479.77777777777783</v>
       </c>
       <c r="C126" s="1">
+        <f t="shared" si="2"/>
         <v>119809.17670092999</v>
       </c>
       <c r="D126" s="1">
+        <f t="shared" si="3"/>
         <v>31320.823299069998</v>
       </c>
       <c r="E126" s="1">
@@ -4830,13 +5275,13 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M126" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="O126" s="1">
         <v>2605</v>
       </c>
       <c r="P126" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:16">
@@ -4847,9 +5292,11 @@
         <v>324.5555555555556</v>
       </c>
       <c r="C127" s="1">
+        <f t="shared" si="2"/>
         <v>124110.31707184424</v>
       </c>
       <c r="D127" s="1">
+        <f t="shared" si="3"/>
         <v>32445.238483711324</v>
       </c>
       <c r="E127" s="1">
@@ -4865,13 +5312,13 @@
         <v>0.79275575134605969</v>
       </c>
       <c r="M127" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O127" s="1">
         <v>2692</v>
       </c>
       <c r="P127" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="128" spans="1:16">
@@ -4882,9 +5329,11 @@
         <v>282.22222222222223</v>
       </c>
       <c r="C128" s="1">
+        <f t="shared" si="2"/>
         <v>127638.5328825984</v>
       </c>
       <c r="D128" s="1">
+        <f t="shared" si="3"/>
         <v>34028.133784068261</v>
       </c>
       <c r="E128" s="1">
@@ -4900,13 +5349,13 @@
         <v>0.78951669824287674</v>
       </c>
       <c r="M128" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O128" s="1">
         <v>2874</v>
       </c>
       <c r="P128" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="129" spans="1:16">
@@ -4917,9 +5366,11 @@
         <v>225.7777777777778</v>
       </c>
       <c r="C129" s="1">
+        <f t="shared" si="2"/>
         <v>135147.90554684089</v>
       </c>
       <c r="D129" s="1">
+        <f t="shared" si="3"/>
         <v>35629.87223093689</v>
       </c>
       <c r="E129" s="1">
@@ -4935,13 +5386,13 @@
         <v>0.79136704614285491</v>
       </c>
       <c r="M129" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O129" s="1">
         <v>3274</v>
       </c>
       <c r="P129" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="130" spans="1:16">
@@ -4952,9 +5403,11 @@
         <v>155.2222222222222</v>
       </c>
       <c r="C130" s="1">
+        <f t="shared" si="2"/>
         <v>129309.45847250981</v>
       </c>
       <c r="D130" s="1">
+        <f t="shared" si="3"/>
         <v>34801.652638601285</v>
       </c>
       <c r="E130" s="1">
@@ -4970,13 +5423,13 @@
         <v>0.78793847410466378</v>
       </c>
       <c r="M130" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O130" s="1">
         <v>3304</v>
       </c>
       <c r="P130" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:16">
@@ -4987,9 +5440,11 @@
         <v>56.44444444444445</v>
       </c>
       <c r="C131" s="1">
+        <f t="shared" si="2"/>
         <v>118108.88873303669</v>
       </c>
       <c r="D131" s="1">
+        <f t="shared" si="3"/>
         <v>35446.666822518848</v>
       </c>
       <c r="E131" s="1">
@@ -5005,13 +5460,13 @@
         <v>0.76916063574336491</v>
       </c>
       <c r="M131" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O131" s="1">
         <v>3072</v>
       </c>
       <c r="P131" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="132" spans="1:16">
@@ -5022,9 +5477,11 @@
         <v>42.333333333333336</v>
       </c>
       <c r="C132" s="1">
+        <f t="shared" si="2"/>
         <v>121122.1162072357</v>
       </c>
       <c r="D132" s="1">
+        <f t="shared" si="3"/>
         <v>36766.772681653179</v>
       </c>
       <c r="E132" s="1">
@@ -5040,13 +5497,13 @@
         <v>0.76713514839206287</v>
       </c>
       <c r="M132" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O132" s="1">
         <v>3366</v>
       </c>
       <c r="P132" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:16">
@@ -5057,9 +5514,11 @@
         <v>28.222222222222225</v>
       </c>
       <c r="C133" s="1">
+        <f t="shared" si="2"/>
         <v>118979.10907694658</v>
       </c>
       <c r="D133" s="1">
+        <f t="shared" si="3"/>
         <v>37354.224256386726</v>
       </c>
       <c r="E133" s="1">
@@ -5075,13 +5534,13 @@
         <v>0.76106039921287805</v>
       </c>
       <c r="M133" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O133" s="1">
         <v>3468</v>
       </c>
       <c r="P133" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:16">
@@ -5092,9 +5551,11 @@
         <v>14.111111111111112</v>
       </c>
       <c r="C134" s="1">
+        <f t="shared" ref="C134:C168" si="4">$E134*($L134)</f>
         <v>118342.18676908125</v>
       </c>
       <c r="D134" s="1">
+        <f t="shared" ref="D134:D168" si="5">$E134*(1-$L134)</f>
         <v>38768.924342029874</v>
       </c>
       <c r="E134" s="1">
@@ -5110,13 +5571,13 @@
         <v>0.75323881253304892</v>
       </c>
       <c r="M134" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O134" s="1">
         <v>3550</v>
       </c>
       <c r="P134" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="135" spans="1:16">
@@ -5127,9 +5588,11 @@
         <v>4</v>
       </c>
       <c r="C135" s="1">
+        <f t="shared" si="4"/>
         <v>123792.55068896992</v>
       </c>
       <c r="D135" s="1">
+        <f t="shared" si="5"/>
         <v>39020.782644363419</v>
       </c>
       <c r="E135" s="1">
@@ -5145,13 +5608,13 @@
         <v>0.76033423156766389</v>
       </c>
       <c r="M135" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O135" s="1">
         <v>3828</v>
       </c>
       <c r="P135" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:16">
@@ -5162,9 +5625,11 @@
         <v>11</v>
       </c>
       <c r="C136" s="1">
+        <f t="shared" si="4"/>
         <v>121376.73001342786</v>
       </c>
       <c r="D136" s="1">
+        <f t="shared" si="5"/>
         <v>37597.714431016575</v>
       </c>
       <c r="E136" s="1">
@@ -5180,13 +5645,13 @@
         <v>0.76349837508533924</v>
       </c>
       <c r="M136" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O136" s="1">
         <v>3704</v>
       </c>
       <c r="P136" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="137" spans="1:16">
@@ -5197,9 +5662,11 @@
         <v>9</v>
       </c>
       <c r="C137" s="1">
+        <f t="shared" si="4"/>
         <v>110285.03474489234</v>
       </c>
       <c r="D137" s="1">
+        <f t="shared" si="5"/>
         <v>37992.743032885439</v>
       </c>
       <c r="E137" s="1">
@@ -5215,13 +5682,13 @@
         <v>0.74377318299290451</v>
       </c>
       <c r="M137" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O137" s="1">
         <v>3555</v>
       </c>
       <c r="P137" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:16">
@@ -5232,9 +5699,11 @@
         <v>1</v>
       </c>
       <c r="C138" s="1">
+        <f t="shared" si="4"/>
         <v>97526.139920868314</v>
       </c>
       <c r="D138" s="1">
+        <f t="shared" si="5"/>
         <v>38249.415634687219</v>
       </c>
       <c r="E138" s="1">
@@ -5250,13 +5719,13 @@
         <v>0.71828938222214356</v>
       </c>
       <c r="M138" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O138" s="1">
         <v>3273</v>
       </c>
       <c r="P138" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="139" spans="1:16">
@@ -5267,9 +5736,11 @@
         <v>1</v>
       </c>
       <c r="C139" s="1">
+        <f t="shared" si="4"/>
         <v>90493.172556167352</v>
       </c>
       <c r="D139" s="1">
+        <f t="shared" si="5"/>
         <v>37064.605221610429</v>
       </c>
       <c r="E139" s="1">
@@ -5285,13 +5756,13 @@
         <v>0.70942888887432809</v>
       </c>
       <c r="M139" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O139" s="1">
         <v>3231</v>
       </c>
       <c r="P139" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="140" spans="1:16">
@@ -5302,9 +5773,11 @@
         <v>1</v>
       </c>
       <c r="C140" s="1">
+        <f t="shared" si="4"/>
         <v>91490.74377563961</v>
       </c>
       <c r="D140" s="1">
+        <f t="shared" si="5"/>
         <v>39569.256224360397</v>
       </c>
       <c r="E140" s="1">
@@ -5320,13 +5793,13 @@
         <v>0.69808289161940795</v>
       </c>
       <c r="M140" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O140" s="1">
         <v>3364</v>
       </c>
       <c r="P140" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="141" spans="1:16">
@@ -5337,9 +5810,11 @@
         <v>0</v>
       </c>
       <c r="C141" s="1">
+        <f t="shared" si="4"/>
         <v>95693.405678297262</v>
       </c>
       <c r="D141" s="1">
+        <f t="shared" si="5"/>
         <v>42811.038766147212</v>
       </c>
       <c r="E141" s="1">
@@ -5355,13 +5830,13 @@
         <v>0.69090494577364159</v>
       </c>
       <c r="M141" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O141" s="1">
         <v>3330</v>
       </c>
       <c r="P141" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="142" spans="1:16">
@@ -5372,9 +5847,11 @@
         <v>0</v>
       </c>
       <c r="C142" s="1">
+        <f t="shared" si="4"/>
         <v>102060.01303317322</v>
       </c>
       <c r="D142" s="1">
+        <f t="shared" si="5"/>
         <v>42821.702670032719</v>
       </c>
       <c r="E142" s="1">
@@ -5386,17 +5863,20 @@
       <c r="G142" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J142" s="1">
+        <v>144881.71570320593</v>
+      </c>
       <c r="L142" s="2">
         <v>0.70443680583025314</v>
       </c>
       <c r="M142" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O142" s="1">
         <v>3385</v>
       </c>
       <c r="P142" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:16">
@@ -5407,9 +5887,11 @@
         <v>0</v>
       </c>
       <c r="C143" s="1">
+        <f t="shared" si="4"/>
         <v>98747.008470234185</v>
       </c>
       <c r="D143" s="1">
+        <f t="shared" si="5"/>
         <v>50777.279531775406</v>
       </c>
       <c r="E143" s="1">
@@ -5421,17 +5903,20 @@
       <c r="G143" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J143" s="1">
+        <v>149524.28800200959</v>
+      </c>
       <c r="L143" s="2">
         <v>0.66040781594564113</v>
       </c>
       <c r="M143" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O143" s="1">
         <v>3505</v>
       </c>
       <c r="P143" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="144" spans="1:16">
@@ -5442,9 +5927,11 @@
         <v>0</v>
       </c>
       <c r="C144" s="1">
+        <f t="shared" si="4"/>
         <v>102715.21620750133</v>
       </c>
       <c r="D144" s="1">
+        <f t="shared" si="5"/>
         <v>57254.85946681651</v>
       </c>
       <c r="E144" s="1">
@@ -5456,17 +5943,20 @@
       <c r="G144" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J144" s="1">
+        <v>159970.07567431784</v>
+      </c>
       <c r="L144" s="2">
         <v>0.64209018952156183</v>
       </c>
       <c r="M144" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O144" s="1">
         <v>3735</v>
       </c>
       <c r="P144" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="145" spans="1:16">
@@ -5477,9 +5967,11 @@
         <v>0</v>
       </c>
       <c r="C145" s="1">
+        <f t="shared" si="4"/>
         <v>106816.86042414946</v>
       </c>
       <c r="D145" s="1">
+        <f t="shared" si="5"/>
         <v>64508.696143188114</v>
       </c>
       <c r="E145" s="1">
@@ -5491,17 +5983,20 @@
       <c r="G145" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J145" s="1">
+        <v>171325.55656733757</v>
+      </c>
       <c r="L145" s="2">
         <v>0.62347300989018706</v>
       </c>
       <c r="M145" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O145" s="1">
         <v>3940</v>
       </c>
       <c r="P145" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="146" spans="1:16">
@@ -5512,9 +6007,11 @@
         <v>0</v>
       </c>
       <c r="C146" s="1">
+        <f t="shared" si="4"/>
         <v>111413.05876254434</v>
       </c>
       <c r="D146" s="1">
+        <f t="shared" si="5"/>
         <v>67608.293327134437</v>
       </c>
       <c r="E146" s="1">
@@ -5526,17 +6023,20 @@
       <c r="G146" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J146" s="1">
+        <v>179021.35208967878</v>
+      </c>
       <c r="L146" s="2">
         <v>0.62234508600255234</v>
       </c>
       <c r="M146" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O146" s="1">
         <v>4008</v>
       </c>
       <c r="P146" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="147" spans="1:16">
@@ -5547,9 +6047,11 @@
         <v>0</v>
       </c>
       <c r="C147" s="1">
+        <f t="shared" si="4"/>
         <v>115347.23664617109</v>
       </c>
       <c r="D147" s="1">
+        <f t="shared" si="5"/>
         <v>71537.210868508453</v>
       </c>
       <c r="E147" s="1">
@@ -5561,17 +6063,20 @@
       <c r="G147" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J147" s="1">
+        <v>186884.44751467954</v>
+      </c>
       <c r="L147" s="2">
         <v>0.61721153461478229</v>
       </c>
       <c r="M147" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O147" s="1">
         <v>4120</v>
       </c>
       <c r="P147" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="148" spans="1:16">
@@ -5582,9 +6087,11 @@
         <v>0</v>
       </c>
       <c r="C148" s="1">
+        <f t="shared" si="4"/>
         <v>126677.73909256482</v>
       </c>
       <c r="D148" s="1">
+        <f t="shared" si="5"/>
         <v>63918.675012374413</v>
       </c>
       <c r="E148" s="1">
@@ -5596,17 +6103,20 @@
       <c r="G148" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J148" s="1">
+        <v>190596.41410493923</v>
+      </c>
       <c r="L148" s="2">
         <v>0.66463862758098979</v>
       </c>
       <c r="M148" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O148" s="1">
         <v>4220</v>
       </c>
       <c r="P148" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="149" spans="1:16">
@@ -5617,9 +6127,11 @@
         <v>0</v>
       </c>
       <c r="C149" s="1">
+        <f t="shared" si="4"/>
         <v>125344.28814290521</v>
       </c>
       <c r="D149" s="1">
+        <f t="shared" si="5"/>
         <v>73261.608801861978</v>
       </c>
       <c r="E149" s="1">
@@ -5631,17 +6143,20 @@
       <c r="G149" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J149" s="1">
+        <v>198605.89694476718</v>
+      </c>
       <c r="L149" s="2">
         <v>0.63112067703490082</v>
       </c>
       <c r="M149" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O149" s="1">
         <v>4330</v>
       </c>
       <c r="P149" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="150" spans="1:16">
@@ -5652,9 +6167,11 @@
         <v>0</v>
       </c>
       <c r="C150" s="1">
+        <f t="shared" si="4"/>
         <v>127661.51424817363</v>
       </c>
       <c r="D150" s="1">
+        <f t="shared" si="5"/>
         <v>77280.866509825573</v>
       </c>
       <c r="E150" s="1">
@@ -5666,17 +6183,20 @@
       <c r="G150" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J150" s="1">
+        <v>204942.3807579992</v>
+      </c>
       <c r="L150" s="2">
         <v>0.62291417605282606</v>
       </c>
       <c r="M150" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O150" s="1">
         <v>4485</v>
       </c>
       <c r="P150" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="151" spans="1:16">
@@ -5687,9 +6207,11 @@
         <v>0</v>
       </c>
       <c r="C151" s="1">
+        <f t="shared" si="4"/>
         <v>128834.12214262012</v>
       </c>
       <c r="D151" s="1">
+        <f t="shared" si="5"/>
         <v>82256.530038119061</v>
       </c>
       <c r="E151" s="1">
@@ -5701,17 +6223,20 @@
       <c r="G151" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J151" s="1">
+        <v>211090.65218073918</v>
+      </c>
       <c r="L151" s="2">
         <v>0.61032604149761349</v>
       </c>
       <c r="M151" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O151" s="1">
         <v>4651</v>
       </c>
       <c r="P151" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="152" spans="1:16">
@@ -5722,9 +6247,11 @@
         <v>0</v>
       </c>
       <c r="C152" s="1">
+        <f t="shared" si="4"/>
         <v>129281.99947537547</v>
       </c>
       <c r="D152" s="1">
+        <f t="shared" si="5"/>
         <v>86932.212224313684</v>
       </c>
       <c r="E152" s="1">
@@ -5736,17 +6263,20 @@
       <c r="G152" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J152" s="1">
+        <v>216214.21169968916</v>
+      </c>
       <c r="L152" s="2">
         <v>0.5979347909606505</v>
       </c>
       <c r="M152" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O152" s="1">
         <v>4758</v>
       </c>
       <c r="P152" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="153" spans="1:16">
@@ -5757,9 +6287,11 @@
         <v>0</v>
       </c>
       <c r="C153" s="1">
+        <f t="shared" si="4"/>
         <v>140256.29564279946</v>
       </c>
       <c r="D153" s="1">
+        <f t="shared" si="5"/>
         <v>87951.227828799136</v>
       </c>
       <c r="E153" s="1">
@@ -5771,17 +6303,20 @@
       <c r="G153" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J153" s="1">
+        <v>228207.5234715986</v>
+      </c>
       <c r="L153" s="2">
         <v>0.61459978842570873</v>
       </c>
       <c r="M153" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O153" s="1">
         <v>4953</v>
       </c>
       <c r="P153" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="154" spans="1:16">
@@ -5792,9 +6327,11 @@
         <v>0</v>
       </c>
       <c r="C154" s="1">
+        <f t="shared" si="4"/>
         <v>136312.43244842952</v>
       </c>
       <c r="D154" s="1">
+        <f t="shared" si="5"/>
         <v>89416.961215023854</v>
       </c>
       <c r="E154" s="1">
@@ -5806,17 +6343,20 @@
       <c r="G154" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J154" s="1">
+        <v>225729.39366345337</v>
+      </c>
       <c r="L154" s="2">
         <v>0.60387542019300222</v>
       </c>
       <c r="M154" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O154" s="1">
         <v>5631</v>
       </c>
       <c r="P154" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="155" spans="1:16">
@@ -5827,9 +6367,11 @@
         <v>0</v>
       </c>
       <c r="C155" s="1">
+        <f t="shared" si="4"/>
         <v>139471.5963928487</v>
       </c>
       <c r="D155" s="1">
+        <f t="shared" si="5"/>
         <v>90555.313520172946</v>
       </c>
       <c r="E155" s="1">
@@ -5841,17 +6383,20 @@
       <c r="G155" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J155" s="1">
+        <v>230026.90991302163</v>
+      </c>
       <c r="L155" s="2">
         <v>0.60632730512089239</v>
       </c>
       <c r="M155" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O155" s="1">
         <v>5683</v>
       </c>
       <c r="P155" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:16">
@@ -5862,9 +6407,11 @@
         <v>0</v>
       </c>
       <c r="C156" s="1">
+        <f t="shared" si="4"/>
         <v>157881.46616490994</v>
       </c>
       <c r="D156" s="1">
+        <f t="shared" si="5"/>
         <v>89858.320942195918</v>
       </c>
       <c r="E156" s="1">
@@ -5876,17 +6423,20 @@
       <c r="G156" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J156" s="1">
+        <v>247739.78710710586</v>
+      </c>
       <c r="L156" s="2">
         <v>0.63728748623107812</v>
       </c>
       <c r="M156" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O156" s="1">
         <v>5984</v>
       </c>
       <c r="P156" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:16">
@@ -5897,9 +6447,11 @@
         <v>0</v>
       </c>
       <c r="C157" s="1">
+        <f t="shared" si="4"/>
         <v>165806.02285185352</v>
       </c>
       <c r="D157" s="1">
+        <f t="shared" si="5"/>
         <v>84004.100550664763</v>
       </c>
       <c r="E157" s="1">
@@ -5911,17 +6463,20 @@
       <c r="G157" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J157" s="1">
+        <v>249810.12340251828</v>
+      </c>
       <c r="L157" s="2">
         <v>0.66372819721437304</v>
       </c>
       <c r="M157" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O157" s="1">
         <v>6020</v>
       </c>
       <c r="P157" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="158" spans="1:16">
@@ -5932,9 +6487,11 @@
         <v>0</v>
       </c>
       <c r="C158" s="1">
+        <f t="shared" si="4"/>
         <v>160031.64792196627</v>
       </c>
       <c r="D158" s="1">
+        <f t="shared" si="5"/>
         <v>92716.680021011096</v>
       </c>
       <c r="E158" s="1">
@@ -5946,17 +6503,23 @@
       <c r="G158" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J158" s="1">
+        <v>252748.32794297737</v>
+      </c>
+      <c r="K158" t="s">
+        <v>28</v>
+      </c>
       <c r="L158" s="2">
         <v>0.63316600044163718</v>
       </c>
       <c r="M158" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O158" s="1">
         <v>6127</v>
       </c>
       <c r="P158" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="159" spans="1:16">
@@ -5967,9 +6530,11 @@
         <v>0</v>
       </c>
       <c r="C159" s="1">
+        <f t="shared" si="4"/>
         <v>158829.10777446159</v>
       </c>
       <c r="D159" s="1">
+        <f t="shared" si="5"/>
         <v>111402.059996443</v>
       </c>
       <c r="E159" s="1">
@@ -5981,17 +6546,23 @@
       <c r="G159" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J159" s="1">
+        <v>270231.16777090461</v>
+      </c>
+      <c r="K159">
+        <v>1</v>
+      </c>
       <c r="L159" s="2">
         <v>0.58775273438892528</v>
       </c>
       <c r="M159" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O159" s="1">
         <v>6480</v>
       </c>
       <c r="P159" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="160" spans="1:16">
@@ -6002,9 +6573,11 @@
         <v>0</v>
       </c>
       <c r="C160" s="1">
+        <f t="shared" si="4"/>
         <v>170498.32544699695</v>
       </c>
       <c r="D160" s="1">
+        <f t="shared" si="5"/>
         <v>118459.97517786566</v>
       </c>
       <c r="E160" s="1">
@@ -6016,17 +6589,23 @@
       <c r="G160" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J160" s="1">
+        <v>288958.3006248626</v>
+      </c>
+      <c r="K160">
+        <v>1</v>
+      </c>
       <c r="L160" s="2">
         <v>0.5900447402905542</v>
       </c>
       <c r="M160" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O160" s="1">
         <v>6758</v>
       </c>
       <c r="P160" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="161" spans="1:16">
@@ -6037,9 +6616,11 @@
         <v>0</v>
       </c>
       <c r="C161" s="1">
+        <f t="shared" si="4"/>
         <v>189903.46068584552</v>
       </c>
       <c r="D161" s="1">
+        <f t="shared" si="5"/>
         <v>114310.49981278856</v>
       </c>
       <c r="E161" s="1">
@@ -6051,17 +6632,23 @@
       <c r="G161" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="J161" s="1">
+        <v>304213.96049863409</v>
+      </c>
+      <c r="K161">
+        <v>1</v>
+      </c>
       <c r="L161" s="2">
         <v>0.6242430833041871</v>
       </c>
       <c r="M161" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O161" s="1">
         <v>7109</v>
       </c>
       <c r="P161" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="162" spans="1:16">
@@ -6072,13 +6659,16 @@
         <v>0</v>
       </c>
       <c r="C162" s="1">
-        <v>195606.11350732695</v>
+        <f t="shared" si="4"/>
+        <v>201186.46809687535</v>
       </c>
       <c r="D162" s="1">
-        <v>125254.18730593644</v>
+        <f t="shared" si="5"/>
+        <v>128827.50496181152</v>
       </c>
       <c r="E162" s="1">
-        <v>320860.3008132634</v>
+        <f>J162*K162</f>
+        <v>330013.97305868688</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>6</v>
@@ -6087,19 +6677,26 @@
         <v>11</v>
       </c>
       <c r="I162" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="J162" s="1">
+        <v>320860.3008132634</v>
+      </c>
+      <c r="K162">
+        <f>1+(K163-1)/2</f>
+        <v>1.0285285285285286</v>
       </c>
       <c r="L162" s="2">
         <v>0.60963015060304149</v>
       </c>
       <c r="M162" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O162" s="1">
         <v>7700.3348957699</v>
       </c>
       <c r="P162" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="163" spans="1:16">
@@ -6110,34 +6707,44 @@
         <v>0</v>
       </c>
       <c r="C163" s="1">
-        <v>199172.25987019532</v>
+        <f t="shared" si="4"/>
+        <v>210536.44286579205</v>
       </c>
       <c r="D163" s="1">
-        <v>133827.74012980468</v>
+        <f t="shared" si="5"/>
+        <v>141463.55713420795</v>
       </c>
       <c r="E163" s="1">
-        <v>333000</v>
+        <f>I163</f>
+        <v>352000</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I163" s="1">
         <v>352000</v>
       </c>
+      <c r="J163" s="1">
+        <v>333000</v>
+      </c>
+      <c r="K163">
+        <f>I163/J163</f>
+        <v>1.057057057057057</v>
+      </c>
       <c r="L163" s="2">
         <v>0.59811489450509103</v>
       </c>
       <c r="M163" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O163" s="1">
         <v>8034.0740245856996</v>
       </c>
       <c r="P163" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="164" spans="1:16">
@@ -6148,13 +6755,16 @@
         <v>0</v>
       </c>
       <c r="C164" s="1">
-        <v>205919.36055308135</v>
+        <f t="shared" si="4"/>
+        <v>217668.51325731122</v>
       </c>
       <c r="D164" s="1">
-        <v>137486.88944691865</v>
+        <f t="shared" si="5"/>
+        <v>145331.48674268878</v>
       </c>
       <c r="E164" s="1">
-        <v>343406.25</v>
+        <f>I164</f>
+        <v>363000</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>6</v>
@@ -6169,13 +6779,13 @@
         <v>0.59963777756835046</v>
       </c>
       <c r="M164" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O164" s="1">
         <v>8229.4987638914008</v>
       </c>
       <c r="P164" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="165" spans="1:16">
@@ -6186,13 +6796,16 @@
         <v>0</v>
       </c>
       <c r="C165" s="1">
-        <v>176694.84690932513</v>
+        <f t="shared" si="4"/>
+        <v>186776.53487111846</v>
       </c>
       <c r="D165" s="1">
-        <v>119410.2667270385</v>
+        <f t="shared" si="5"/>
+        <v>126223.46512888154</v>
       </c>
       <c r="E165" s="1">
-        <v>296105.11363636365</v>
+        <f t="shared" ref="E165:E168" si="6">I165</f>
+        <v>313000</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>6</v>
@@ -6207,13 +6820,13 @@
         <v>0.59673014335820596</v>
       </c>
       <c r="M165" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O165" s="1">
         <v>7857.999159895</v>
       </c>
       <c r="P165" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="166" spans="1:16">
@@ -6224,13 +6837,16 @@
         <v>0</v>
       </c>
       <c r="C166" s="1">
-        <v>159141.42984236317</v>
+        <f t="shared" si="4"/>
+        <v>168221.57148502051</v>
       </c>
       <c r="D166" s="1">
-        <v>118043.22924854595</v>
+        <f t="shared" si="5"/>
+        <v>124778.42851497949</v>
       </c>
       <c r="E166" s="1">
-        <v>277184.65909090912</v>
+        <f t="shared" si="6"/>
+        <v>293000</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>6</v>
@@ -6245,13 +6861,13 @@
         <v>0.57413505626286865</v>
       </c>
       <c r="M166" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O166" s="1">
         <v>8408.9027169411002</v>
       </c>
       <c r="P166" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="167" spans="1:16">
@@ -6262,13 +6878,16 @@
         <v>0</v>
       </c>
       <c r="C167" s="1">
-        <v>177608.35344181827</v>
+        <f t="shared" si="4"/>
+        <v>187742.16339795804</v>
       </c>
       <c r="D167" s="1">
-        <v>131741.07837636356</v>
+        <f t="shared" si="5"/>
+        <v>139257.83660204196</v>
       </c>
       <c r="E167" s="1">
-        <v>309349.43181818182</v>
+        <f t="shared" si="6"/>
+        <v>327000</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>6</v>
@@ -6283,13 +6902,13 @@
         <v>0.57413505626286865</v>
       </c>
       <c r="M167" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="O167" s="1">
         <v>8784.2649371619009</v>
       </c>
       <c r="P167" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="168" spans="1:16">
@@ -6300,13 +6919,16 @@
         <v>0</v>
       </c>
       <c r="C168" s="1">
-        <v>162943.44352460391</v>
+        <f t="shared" si="4"/>
+        <v>172240.5168788606</v>
       </c>
       <c r="D168" s="1">
-        <v>120863.37465721427</v>
+        <f t="shared" si="5"/>
+        <v>127759.4831211394</v>
       </c>
       <c r="E168" s="1">
-        <v>283806.81818181818</v>
+        <f t="shared" si="6"/>
+        <v>300000</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>6</v>
@@ -6321,13 +6943,13 @@
         <v>0.57413505626286865</v>
       </c>
       <c r="M168" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="O168" s="1">
         <v>9196.7031038762998</v>
       </c>
       <c r="P168" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="169" spans="1:16">
@@ -54989,6 +55611,53 @@
     </row>
     <row r="16388" spans="7:7">
       <c r="G16388" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added extrapolation for VOCs from crude oil loading and transport
</commit_message>
<xml_diff>
--- a/input/energy/Shipping_Fuel_Consumption.xlsx
+++ b/input/energy/Shipping_Fuel_Consumption.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="22620" windowHeight="18960" tabRatio="500"/>
+    <workbookView xWindow="1820" yWindow="2860" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="References" sheetId="2" r:id="rId2"/>
+    <sheet name="Crude_Oil_Loaded" sheetId="3" r:id="rId2"/>
+    <sheet name="References" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="121">
   <si>
     <t>Year</t>
   </si>
@@ -181,12 +182,273 @@
   <si>
     <t>Smith, SJ, J van Aardenne, Z Klimont, R Andres, AC Volke, and S Delgado Arias (2011) Anthropogenic Sulfur Dioxide Emissions: 1850-2005 Atmos. Chem. Phys., 11, 1101–1116.</t>
   </si>
+  <si>
+    <t>Crude Oil loaded</t>
+  </si>
+  <si>
+    <t>World seaborne trade by types of cargo and country groups, annual, 1970-2014</t>
+  </si>
+  <si>
+    <t>UNCTAD, UNCTADstat</t>
+  </si>
+  <si>
+    <t>Downloaded:</t>
+  </si>
+  <si>
+    <t>MEASURE</t>
+  </si>
+  <si>
+    <t>Metric tons in millions</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>CDIAC_Petr_CO2</t>
+  </si>
+  <si>
+    <t>Extrapolated</t>
+  </si>
+  <si>
+    <t>(IMO GHG study 2014)</t>
+  </si>
+  <si>
+    <t>Crude Oil Tanker VOC Losses</t>
+  </si>
+  <si>
+    <t>Tanker Loss:</t>
+  </si>
+  <si>
+    <t>CEDS Input Format</t>
+  </si>
+  <si>
+    <t>iso</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>2L_Other-process-emissions</t>
+  </si>
+  <si>
+    <t>X1960</t>
+  </si>
+  <si>
+    <t>X1961</t>
+  </si>
+  <si>
+    <t>X1962</t>
+  </si>
+  <si>
+    <t>X1963</t>
+  </si>
+  <si>
+    <t>X1964</t>
+  </si>
+  <si>
+    <t>X1965</t>
+  </si>
+  <si>
+    <t>X1966</t>
+  </si>
+  <si>
+    <t>X1967</t>
+  </si>
+  <si>
+    <t>X1968</t>
+  </si>
+  <si>
+    <t>X1969</t>
+  </si>
+  <si>
+    <t>X1970</t>
+  </si>
+  <si>
+    <t>X1971</t>
+  </si>
+  <si>
+    <t>X1972</t>
+  </si>
+  <si>
+    <t>X1973</t>
+  </si>
+  <si>
+    <t>X1974</t>
+  </si>
+  <si>
+    <t>X1975</t>
+  </si>
+  <si>
+    <t>X1976</t>
+  </si>
+  <si>
+    <t>X1977</t>
+  </si>
+  <si>
+    <t>X1978</t>
+  </si>
+  <si>
+    <t>X1979</t>
+  </si>
+  <si>
+    <t>X1980</t>
+  </si>
+  <si>
+    <t>X1981</t>
+  </si>
+  <si>
+    <t>X1982</t>
+  </si>
+  <si>
+    <t>X1983</t>
+  </si>
+  <si>
+    <t>X1984</t>
+  </si>
+  <si>
+    <t>X1985</t>
+  </si>
+  <si>
+    <t>X1986</t>
+  </si>
+  <si>
+    <t>X1987</t>
+  </si>
+  <si>
+    <t>X1988</t>
+  </si>
+  <si>
+    <t>X1989</t>
+  </si>
+  <si>
+    <t>X1990</t>
+  </si>
+  <si>
+    <t>X1991</t>
+  </si>
+  <si>
+    <t>X1992</t>
+  </si>
+  <si>
+    <t>X1993</t>
+  </si>
+  <si>
+    <t>X1994</t>
+  </si>
+  <si>
+    <t>X1995</t>
+  </si>
+  <si>
+    <t>X1996</t>
+  </si>
+  <si>
+    <t>X1997</t>
+  </si>
+  <si>
+    <t>X1998</t>
+  </si>
+  <si>
+    <t>X1999</t>
+  </si>
+  <si>
+    <t>X2000</t>
+  </si>
+  <si>
+    <t>X2001</t>
+  </si>
+  <si>
+    <t>X2002</t>
+  </si>
+  <si>
+    <t>X2003</t>
+  </si>
+  <si>
+    <t>X2004</t>
+  </si>
+  <si>
+    <t>X2005</t>
+  </si>
+  <si>
+    <t>X2006</t>
+  </si>
+  <si>
+    <t>X2007</t>
+  </si>
+  <si>
+    <t>X2008</t>
+  </si>
+  <si>
+    <t>X2009</t>
+  </si>
+  <si>
+    <t>X2010</t>
+  </si>
+  <si>
+    <t>X2011</t>
+  </si>
+  <si>
+    <t>X2012</t>
+  </si>
+  <si>
+    <t>X2013</t>
+  </si>
+  <si>
+    <t>X2014</t>
+  </si>
+  <si>
+    <t>CEDS Metadata</t>
+  </si>
+  <si>
+    <t>Data.Type</t>
+  </si>
+  <si>
+    <t>Emission</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Start.Year</t>
+  </si>
+  <si>
+    <t>End.Year</t>
+  </si>
+  <si>
+    <t>Source.Comment</t>
+  </si>
+  <si>
+    <t>Emissions</t>
+  </si>
+  <si>
+    <t>NMVOC</t>
+  </si>
+  <si>
+    <t>crude oil loading</t>
+  </si>
+  <si>
+    <t>IMO GHG study (2014) scaled by crude oil transport from UNCTAD until 1970, then by CDIAC CO2 from petroleum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -225,6 +487,19 @@
       <name val="Times"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,7 +518,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -297,8 +572,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -310,8 +639,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -338,6 +676,33 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -364,6 +729,33 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,11 +1087,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FH16388"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G159" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5:G9"/>
+      <selection pane="bottomRight" activeCell="R5" sqref="R5:S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -55626,6 +56018,1501 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BS60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5:BS6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="46" width="6.6640625" customWidth="1"/>
+    <col min="47" max="73" width="6.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:71">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" ht="12" customHeight="1">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71" ht="12" customHeight="1">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="7">
+        <v>42014</v>
+      </c>
+      <c r="D3">
+        <v>2012</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2410</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q3">
+        <v>1960</v>
+      </c>
+      <c r="R3">
+        <v>2014</v>
+      </c>
+      <c r="S3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:71" ht="12" customHeight="1">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" t="s">
+        <v>57</v>
+      </c>
+      <c r="U5" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W5" t="s">
+        <v>60</v>
+      </c>
+      <c r="X5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>90</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>92</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>94</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>95</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>96</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>97</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>98</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>99</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>100</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>101</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>102</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>103</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>104</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>105</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>106</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71">
+      <c r="A6" s="8">
+        <v>1960</v>
+      </c>
+      <c r="B6" s="11">
+        <f t="shared" ref="B6:B14" si="0">C6*AVERAGE($F$16:$F$20)/1000</f>
+        <v>536.99612620371681</v>
+      </c>
+      <c r="C6" s="1">
+        <v>774504.00000000012</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6">
+        <f>$F$3*B6/LOOKUP($D$3,$A$6:$A$60,$B$6:$B$60)</f>
+        <v>724.73811885833118</v>
+      </c>
+      <c r="M6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <f>LOOKUP(RIGHT(Q5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>724.73811885833118</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R10" si="1">LOOKUP(RIGHT(R5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>765.89872698200952</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S10" si="2">LOOKUP(RIGHT(S5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>827.15164823528573</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6:T10" si="3">LOOKUP(RIGHT(T5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>890.08984593912112</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ref="U6:U10" si="4">LOOKUP(RIGHT(U5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>957.53739801011068</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:V10" si="5">LOOKUP(RIGHT(V5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1034.173028630817</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ref="W6:W10" si="6">LOOKUP(RIGHT(W5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1114.2596862085818</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ref="X6:X10" si="7">LOOKUP(RIGHT(X5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1188.3266972530616</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ref="Y6:Y10" si="8">LOOKUP(RIGHT(Y5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1299.5914370385883</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z10" si="9">LOOKUP(RIGHT(Z5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1409.7052106752051</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" ref="AA6:AA10" si="10">LOOKUP(RIGHT(AA5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1628.985511769137</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" ref="AB6:AB10" si="11">LOOKUP(RIGHT(AB5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1633.034357283062</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" ref="AC6:AC10" si="12">LOOKUP(RIGHT(AC5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1782.8416412982851</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" ref="AD6:AD10" si="13">LOOKUP(RIGHT(AD5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2043.3173693607901</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6:AE10" si="14">LOOKUP(RIGHT(AE5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2020.3739114485486</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" ref="AF6:AF10" si="15">LOOKUP(RIGHT(AF5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1840.8750936645426</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" ref="AG6:AG10" si="16">LOOKUP(RIGHT(AG5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2098.651591384431</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" ref="AH6:AH10" si="17">LOOKUP(RIGHT(AH5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2158.0346589219967</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" ref="AI6:AI10" si="18">LOOKUP(RIGHT(AI5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2164.7827347785383</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" ref="AJ6:AJ10" si="19">LOOKUP(RIGHT(AJ5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2328.0861705068446</v>
+      </c>
+      <c r="AK6">
+        <f t="shared" ref="AK6:AK10" si="20">LOOKUP(RIGHT(AK5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2060.8623665877981</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" ref="AL6:AL10" si="21">LOOKUP(RIGHT(AL5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1840.8750936645426</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" ref="AM6:AM10" si="22">LOOKUP(RIGHT(AM5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1569.6024442315711</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" ref="AN6:AN10" si="23">LOOKUP(RIGHT(AN5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1442.7386181285895</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" ref="AO6:AO10" si="24">LOOKUP(RIGHT(AO5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1456.2347698416727</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" ref="AP6:AP10" si="25">LOOKUP(RIGHT(AP5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1415.7463147024232</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" ref="AQ6:AQ10" si="26">LOOKUP(RIGHT(AQ5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1519.6666828931634</v>
+      </c>
+      <c r="AR6">
+        <f t="shared" ref="AR6:AR10" si="27">LOOKUP(RIGHT(AR5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1494.0239946383056</v>
+      </c>
+      <c r="AS6">
+        <f t="shared" ref="AS6:AS10" si="28">LOOKUP(RIGHT(AS5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1565.5535987176463</v>
+      </c>
+      <c r="AT6">
+        <f t="shared" ref="AT6:AT10" si="29">LOOKUP(RIGHT(AT5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1700.5151158484778</v>
+      </c>
+      <c r="AU6">
+        <f t="shared" ref="AU6:AU10" si="30">LOOKUP(RIGHT(AU5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1736.9547254738022</v>
+      </c>
+      <c r="AV6">
+        <f t="shared" ref="AV6:AV10" si="31">LOOKUP(RIGHT(AV5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1799.0370233539848</v>
+      </c>
+      <c r="AW6">
+        <f t="shared" ref="AW6:AW10" si="32">LOOKUP(RIGHT(AW5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1881.3635488037921</v>
+      </c>
+      <c r="AX6">
+        <f t="shared" ref="AX6:AX10" si="33">LOOKUP(RIGHT(AX5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>1947.4946921978994</v>
+      </c>
+      <c r="AY6">
+        <f t="shared" ref="AY6:AY10" si="34">LOOKUP(RIGHT(AY5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2021.723526619857</v>
+      </c>
+      <c r="AZ6">
+        <f t="shared" ref="AZ6:AZ10" si="35">LOOKUP(RIGHT(AZ5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2067.6104424443397</v>
+      </c>
+      <c r="BA6">
+        <f t="shared" ref="BA6:BA10" si="36">LOOKUP(RIGHT(BA5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2145.8881223802218</v>
+      </c>
+      <c r="BB6">
+        <f t="shared" ref="BB6:BB10" si="37">LOOKUP(RIGHT(BB5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2194.4742685473211</v>
+      </c>
+      <c r="BC6">
+        <f t="shared" ref="BC6:BC10" si="38">LOOKUP(RIGHT(BC5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2089.2042851852725</v>
+      </c>
+      <c r="BD6">
+        <f t="shared" ref="BD6:BD10" si="39">LOOKUP(RIGHT(BD5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2095.9523610418141</v>
+      </c>
+      <c r="BE6">
+        <f t="shared" ref="BE6:BE10" si="40">LOOKUP(RIGHT(BE5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2166.1323499498467</v>
+      </c>
+      <c r="BF6">
+        <f t="shared" ref="BF6:BF10" si="41">LOOKUP(RIGHT(BF5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2264.6542574553537</v>
+      </c>
+      <c r="BG6">
+        <f t="shared" ref="BG6:BG10" si="42">LOOKUP(RIGHT(BG5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2209.3200354317128</v>
+      </c>
+      <c r="BH6">
+        <f t="shared" ref="BH6:BH10" si="43">LOOKUP(RIGHT(BH5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2280.8496395110537</v>
+      </c>
+      <c r="BI6">
+        <f t="shared" ref="BI6:BI10" si="44">LOOKUP(RIGHT(BI5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2388.8188532157187</v>
+      </c>
+      <c r="BJ6">
+        <f t="shared" ref="BJ6:BJ10" si="45">LOOKUP(RIGHT(BJ5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2506.2353731195421</v>
+      </c>
+      <c r="BK6">
+        <f t="shared" ref="BK6:BK10" si="46">LOOKUP(RIGHT(BK5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2406.923919684823</v>
+      </c>
+      <c r="BL6">
+        <f t="shared" ref="BL6:BL10" si="47">LOOKUP(RIGHT(BL5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2447.4279659869253</v>
+      </c>
+      <c r="BM6">
+        <f t="shared" ref="BM6:BM10" si="48">LOOKUP(RIGHT(BM5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2409.3794735451474</v>
+      </c>
+      <c r="BN6">
+        <f t="shared" ref="BN6:BN10" si="49">LOOKUP(RIGHT(BN5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2308.5608088774939</v>
+      </c>
+      <c r="BO6">
+        <f t="shared" ref="BO6:BO10" si="50">LOOKUP(RIGHT(BO5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2412.681523391569</v>
+      </c>
+      <c r="BP6">
+        <f t="shared" ref="BP6:BP10" si="51">LOOKUP(RIGHT(BP5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2374.6213862927543</v>
+      </c>
+      <c r="BQ6">
+        <f t="shared" ref="BQ6:BQ10" si="52">LOOKUP(RIGHT(BQ5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2410.0000000000005</v>
+      </c>
+      <c r="BR6">
+        <f t="shared" ref="BR6:BR10" si="53">LOOKUP(RIGHT(BR5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2345.5529253112636</v>
+      </c>
+      <c r="BS6">
+        <f t="shared" ref="BS6:BS10" si="54">LOOKUP(RIGHT(BS5,4)*1,$A$6:$A$60,$H$6:$H$60)</f>
+        <v>2308.2246062421691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71">
+      <c r="A7" s="8">
+        <v>1961</v>
+      </c>
+      <c r="B7" s="11">
+        <f t="shared" si="0"/>
+        <v>567.49415927174857</v>
+      </c>
+      <c r="C7" s="1">
+        <v>818491.00000000012</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H60" si="55">$F$3*B7/LOOKUP($D$3,$A$6:$A$60,$B$6:$B$60)</f>
+        <v>765.89872698200952</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71">
+      <c r="A8" s="8">
+        <v>1962</v>
+      </c>
+      <c r="B8" s="11">
+        <f t="shared" si="0"/>
+        <v>612.87963103841344</v>
+      </c>
+      <c r="C8" s="1">
+        <v>883949.99999999988</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="55"/>
+        <v>827.15164823528573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71">
+      <c r="A9" s="8">
+        <v>1963</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" si="0"/>
+        <v>659.51381168623709</v>
+      </c>
+      <c r="C9" s="1">
+        <v>951210</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="55"/>
+        <v>890.08984593912112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71">
+      <c r="A10" s="8">
+        <v>1964</v>
+      </c>
+      <c r="B10" s="11">
+        <f t="shared" si="0"/>
+        <v>709.48920726926531</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1023289</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="55"/>
+        <v>957.53739801011068</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71">
+      <c r="A11" s="8">
+        <v>1965</v>
+      </c>
+      <c r="B11" s="11">
+        <f t="shared" si="0"/>
+        <v>766.27252761858824</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1105187</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="55"/>
+        <v>1034.173028630817</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71">
+      <c r="A12" s="8">
+        <v>1966</v>
+      </c>
+      <c r="B12" s="11">
+        <f t="shared" si="0"/>
+        <v>825.61289313932321</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1190773</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="55"/>
+        <v>1114.2596862085818</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71">
+      <c r="A13" s="8">
+        <v>1967</v>
+      </c>
+      <c r="B13" s="11">
+        <f t="shared" si="0"/>
+        <v>880.49298979137779</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1269926.0000000002</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="55"/>
+        <v>1188.3266972530616</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71">
+      <c r="A14" s="8">
+        <v>1968</v>
+      </c>
+      <c r="B14" s="11">
+        <f t="shared" si="0"/>
+        <v>962.93481628453071</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1388831</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="55"/>
+        <v>1299.5914370385883</v>
+      </c>
+    </row>
+    <row r="15" spans="1:71">
+      <c r="A15" s="8">
+        <v>1969</v>
+      </c>
+      <c r="B15" s="11">
+        <f>C15*AVERAGE($F$16:$F$20)/1000</f>
+        <v>1044.5238321592356</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1506506</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="55"/>
+        <v>1409.7052106752051</v>
+      </c>
+    </row>
+    <row r="16" spans="1:71">
+      <c r="A16" s="8">
+        <v>1970</v>
+      </c>
+      <c r="B16">
+        <v>1207</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1724547</v>
+      </c>
+      <c r="F16" s="9">
+        <f>B16/C16*1000</f>
+        <v>0.6998939431630451</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="55"/>
+        <v>1628.985511769137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="8">
+        <v>1971</v>
+      </c>
+      <c r="B17">
+        <v>1210</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1826256</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" ref="F17:F38" si="56">B17/C17*1000</f>
+        <v>0.66255771370497896</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="55"/>
+        <v>1633.034357283062</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="8">
+        <v>1972</v>
+      </c>
+      <c r="B18">
+        <v>1321</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1969761.0000000002</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="56"/>
+        <v>0.67063973751130201</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="55"/>
+        <v>1782.8416412982851</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="8">
+        <v>1973</v>
+      </c>
+      <c r="B19">
+        <v>1514</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2110972</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="56"/>
+        <v>0.71720515478177826</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="55"/>
+        <v>2043.3173693607901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="8">
+        <v>1974</v>
+      </c>
+      <c r="B20">
+        <v>1497</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2089576.0000000002</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="56"/>
+        <v>0.71641328192896536</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="55"/>
+        <v>2020.3739114485486</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="8">
+        <v>1975</v>
+      </c>
+      <c r="B21">
+        <v>1364</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2073282.9999999998</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="56"/>
+        <v>0.65789378488127292</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="55"/>
+        <v>1840.8750936645426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="8">
+        <v>1976</v>
+      </c>
+      <c r="B22">
+        <v>1555</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2186329.0000000009</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="56"/>
+        <v>0.71123787865412724</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="55"/>
+        <v>2098.651591384431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="8">
+        <v>1977</v>
+      </c>
+      <c r="B23">
+        <v>1599</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2272333</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="56"/>
+        <v>0.70368207476633049</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="55"/>
+        <v>2158.0346589219967</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="8">
+        <v>1978</v>
+      </c>
+      <c r="B24">
+        <v>1604</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2360786.9999999995</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="56"/>
+        <v>0.67943444283622378</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="55"/>
+        <v>2164.7827347785383</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="8">
+        <v>1979</v>
+      </c>
+      <c r="B25">
+        <v>1725</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2399062</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="56"/>
+        <v>0.71903102129082119</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="55"/>
+        <v>2328.0861705068446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="8">
+        <v>1980</v>
+      </c>
+      <c r="B26">
+        <v>1527</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2312198</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" si="56"/>
+        <v>0.66041057037502837</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="55"/>
+        <v>2060.8623665877981</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="8">
+        <v>1981</v>
+      </c>
+      <c r="B27">
+        <v>1364</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2203629.7500000005</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="56"/>
+        <v>0.61897875539209779</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="55"/>
+        <v>1840.8750936645426</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="8">
+        <v>1982</v>
+      </c>
+      <c r="B28">
+        <v>1163</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2158605.5000000005</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="56"/>
+        <v>0.53877375926263493</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="55"/>
+        <v>1569.6024442315711</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="8">
+        <v>1983</v>
+      </c>
+      <c r="B29">
+        <v>1069</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2144851.2500000005</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="56"/>
+        <v>0.4984028612706824</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="55"/>
+        <v>1442.7386181285895</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="8">
+        <v>1984</v>
+      </c>
+      <c r="B30">
+        <v>1079</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2152354.0000000005</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="56"/>
+        <v>0.50131158722031777</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="55"/>
+        <v>1456.2347698416727</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="8">
+        <v>1985</v>
+      </c>
+      <c r="B31">
+        <v>1049</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2153120.9999999991</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" si="56"/>
+        <v>0.48719974399952465</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="55"/>
+        <v>1415.7463147024232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="8">
+        <v>1986</v>
+      </c>
+      <c r="B32">
+        <v>1126</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2218414.9999999995</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="56"/>
+        <v>0.50756959360624598</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="55"/>
+        <v>1519.6666828931634</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="8">
+        <v>1987</v>
+      </c>
+      <c r="B33">
+        <v>1107</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2257766.0000000009</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="56"/>
+        <v>0.49030767581760004</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="55"/>
+        <v>1494.0239946383056</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="8">
+        <v>1988</v>
+      </c>
+      <c r="B34">
+        <v>1160</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2337023.0000000009</v>
+      </c>
+      <c r="F34" s="9">
+        <f t="shared" si="56"/>
+        <v>0.4963579733703945</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="55"/>
+        <v>1565.5535987176463</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="8">
+        <v>1989</v>
+      </c>
+      <c r="B35">
+        <v>1260</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2377288</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="56"/>
+        <v>0.53001571538660852</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="55"/>
+        <v>1700.5151158484778</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="8">
+        <v>1990</v>
+      </c>
+      <c r="B36">
+        <v>1287</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2313094.9999999995</v>
+      </c>
+      <c r="F36" s="9">
+        <f t="shared" si="56"/>
+        <v>0.55639738099818647</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="55"/>
+        <v>1736.9547254738022</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="8">
+        <v>1991</v>
+      </c>
+      <c r="B37">
+        <v>1333</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2453063.9999999995</v>
+      </c>
+      <c r="F37" s="9">
+        <f t="shared" si="56"/>
+        <v>0.54340204739868192</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="55"/>
+        <v>1799.0370233539848</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="8">
+        <v>1992</v>
+      </c>
+      <c r="B38">
+        <v>1394</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2308001</v>
+      </c>
+      <c r="F38" s="9">
+        <f t="shared" si="56"/>
+        <v>0.60398587348965616</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="55"/>
+        <v>1881.3635488037921</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="8">
+        <v>1993</v>
+      </c>
+      <c r="B39">
+        <v>1443</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2321381</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="55"/>
+        <v>1947.4946921978994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="8">
+        <v>1994</v>
+      </c>
+      <c r="B40">
+        <v>1498</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2305699</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="55"/>
+        <v>2021.723526619857</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="8">
+        <v>1995</v>
+      </c>
+      <c r="B41">
+        <v>1532</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2324179</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="55"/>
+        <v>2067.6104424443397</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="8">
+        <v>1996</v>
+      </c>
+      <c r="B42">
+        <v>1590</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2388214</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="55"/>
+        <v>2145.8881223802218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="8">
+        <v>1997</v>
+      </c>
+      <c r="B43">
+        <v>1626</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2412099</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="55"/>
+        <v>2194.4742685473211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="8">
+        <v>1998</v>
+      </c>
+      <c r="B44">
+        <v>1548</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2422764</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="55"/>
+        <v>2089.2042851852725</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="8">
+        <v>1999</v>
+      </c>
+      <c r="B45">
+        <v>1553</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2463389</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="55"/>
+        <v>2095.9523610418141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="8">
+        <v>2000</v>
+      </c>
+      <c r="B46">
+        <v>1605</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2525407</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="55"/>
+        <v>2166.1323499498467</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="8">
+        <v>2001</v>
+      </c>
+      <c r="B47">
+        <v>1678</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2541861</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="55"/>
+        <v>2264.6542574553537</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="8">
+        <v>2002</v>
+      </c>
+      <c r="B48">
+        <v>1637</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2529705</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="55"/>
+        <v>2209.3200354317128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="8">
+        <v>2003</v>
+      </c>
+      <c r="B49">
+        <v>1690</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2601535</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="55"/>
+        <v>2280.8496395110537</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="8">
+        <v>2004</v>
+      </c>
+      <c r="B50">
+        <v>1770</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2680863</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="55"/>
+        <v>2388.8188532157187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="8">
+        <v>2005</v>
+      </c>
+      <c r="B51">
+        <v>1857</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2685411</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="55"/>
+        <v>2506.2353731195421</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="8">
+        <v>2006</v>
+      </c>
+      <c r="B52" s="10">
+        <v>1783.4149844000001</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2697375</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="55"/>
+        <v>2406.923919684823</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="8">
+        <v>2007</v>
+      </c>
+      <c r="B53" s="10">
+        <v>1813.4265367026001</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2694450</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="55"/>
+        <v>2447.4279659869253</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="8">
+        <v>2008</v>
+      </c>
+      <c r="B54" s="10">
+        <v>1785.2344318339999</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2705495</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="55"/>
+        <v>2409.3794735451474</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="8">
+        <v>2009</v>
+      </c>
+      <c r="B55" s="10">
+        <v>1710.5326451240001</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2687981</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="55"/>
+        <v>2308.5608088774939</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="8">
+        <v>2010</v>
+      </c>
+      <c r="B56" s="10">
+        <v>1787.6810921240001</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2736090.5</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="55"/>
+        <v>2412.681523391569</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="8">
+        <v>2011</v>
+      </c>
+      <c r="B57" s="10">
+        <v>1759.480359124</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2711806</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="55"/>
+        <v>2374.6213862927543</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="8">
+        <v>2012</v>
+      </c>
+      <c r="B58" s="10">
+        <v>1785.6942121239999</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="55"/>
+        <v>2410.0000000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="8">
+        <v>2013</v>
+      </c>
+      <c r="B59" s="10">
+        <v>1737.942026124</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="55"/>
+        <v>2345.5529253112636</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="8">
+        <v>2014</v>
+      </c>
+      <c r="B60" s="10">
+        <v>1710.2835351240001</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="55"/>
+        <v>2308.2246062421691</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>